<commit_message>
Test for filter 6 and break out tests
</commit_message>
<xml_diff>
--- a/tests/data/example_masterfile.xlsx
+++ b/tests/data/example_masterfile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiebuntic/projects/RRED/rred-reports/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAB0B48-F120-824A-A57F-F01EED0FC956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1BF5BF-3E94-9945-BFA3-757DA2D69A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="214">
   <si>
     <t>reg_rr_title</t>
   </si>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BC0FAF-0515-DD4A-8720-9B9E6959245E}">
   <dimension ref="A1:BR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
+      <selection activeCell="BJ5" sqref="BJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1066,7 @@
     <col min="29" max="29" width="11" style="2"/>
     <col min="31" max="33" width="11" style="2"/>
     <col min="62" max="62" width="26.5" style="2" customWidth="1"/>
+    <col min="66" max="66" width="38" customWidth="1"/>
     <col min="70" max="70" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1883,8 +1884,8 @@
       <c r="BI4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BJ4" s="2" t="s">
-        <v>69</v>
+      <c r="BJ4" s="2">
+        <v>44629</v>
       </c>
       <c r="BK4" t="s">
         <v>69</v>
@@ -1895,17 +1896,17 @@
       <c r="BM4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BN4" t="s">
-        <v>69</v>
+      <c r="BN4" s="2">
+        <v>44690</v>
       </c>
       <c r="BO4" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="BP4" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="BQ4" s="1" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Read and process masterfile to get date representation columns
</commit_message>
<xml_diff>
--- a/tests/data/example_masterfile.xlsx
+++ b/tests/data/example_masterfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1BF5BF-3E94-9945-BFA3-757DA2D69A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EE6019-0F78-564E-A39E-51B7E5EAEFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
@@ -662,25 +662,25 @@
     <t>Filter Test School</t>
   </si>
   <si>
-    <t>test_5_2021-22</t>
-  </si>
-  <si>
-    <t>test_6_2021-22</t>
-  </si>
-  <si>
     <t>J School</t>
   </si>
   <si>
-    <t>test_1_2021-22</t>
-  </si>
-  <si>
-    <t>test_2_2021-22</t>
-  </si>
-  <si>
-    <t>test_3_2021-22</t>
-  </si>
-  <si>
-    <t>test_4_2021-22</t>
+    <t>test-1_2021-22</t>
+  </si>
+  <si>
+    <t>test-2_2021-22</t>
+  </si>
+  <si>
+    <t>test-3_2021-22</t>
+  </si>
+  <si>
+    <t>test-4_2021-22</t>
+  </si>
+  <si>
+    <t>test-5_2021-22</t>
+  </si>
+  <si>
+    <t>test-6_2021-22</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BC0FAF-0515-DD4A-8720-9B9E6959245E}">
   <dimension ref="A1:BR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BJ5" sqref="BJ5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>187</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>187</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
         <v>187</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
         <v>187</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>187</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
         <v>187</v>
@@ -7575,7 +7575,7 @@
         <v>2030</v>
       </c>
       <c r="F32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>205</v>
@@ -7784,7 +7784,7 @@
         <v>2030</v>
       </c>
       <c r="F33" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>205</v>
@@ -7993,7 +7993,7 @@
         <v>2030</v>
       </c>
       <c r="F34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>205</v>
@@ -8202,7 +8202,7 @@
         <v>2030</v>
       </c>
       <c r="F35" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>205</v>
@@ -8414,7 +8414,7 @@
         <v>2030</v>
       </c>
       <c r="F36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
Use `Left School` as exit outcome for summary table
</commit_message>
<xml_diff>
--- a/tests/data/example_masterfile.xlsx
+++ b/tests/data/example_masterfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/rred-reports/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EE6019-0F78-564E-A39E-51B7E5EAEFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BB9F61-F566-A64E-8D4E-366C638BE162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="215">
   <si>
     <t>reg_rr_title</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>test-6_2021-22</t>
+  </si>
+  <si>
+    <t>Left School</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BC0FAF-0515-DD4A-8720-9B9E6959245E}">
   <dimension ref="A1:BR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1801,7 +1804,7 @@
         <v>44652</v>
       </c>
       <c r="AH4" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="AI4" t="s">
         <v>83</v>
@@ -2219,7 +2222,7 @@
         <v>44974</v>
       </c>
       <c r="AH6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="AI6" t="s">
         <v>83</v>
@@ -2849,7 +2852,7 @@
         <v>69</v>
       </c>
       <c r="AH9" t="s">
-        <v>72</v>
+        <v>214</v>
       </c>
       <c r="AI9" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
changes to example_masterfile adding 2 rred users in 1 school with same pupil_no
</commit_message>
<xml_diff>
--- a/tests/data/example_masterfile.xlsx
+++ b/tests/data/example_masterfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiebuntic/projects/RRED/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BB9F61-F566-A64E-8D4E-366C638BE162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17ED436-6FD4-D343-A477-2DC23E409698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="216">
   <si>
     <t>reg_rr_title</t>
   </si>
@@ -684,6 +684,9 @@
   </si>
   <si>
     <t>Left School</t>
+  </si>
+  <si>
+    <t>AF066XX</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BC0FAF-0515-DD4A-8720-9B9E6959245E}">
-  <dimension ref="A1:BR36"/>
+  <dimension ref="A1:BR41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8612,6 +8615,1057 @@
         <v>157</v>
       </c>
     </row>
+    <row r="37" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>215</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>2030</v>
+      </c>
+      <c r="F37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" t="s">
+        <v>70</v>
+      </c>
+      <c r="J37" t="s">
+        <v>69</v>
+      </c>
+      <c r="K37" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" t="s">
+        <v>69</v>
+      </c>
+      <c r="N37" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" t="s">
+        <v>70</v>
+      </c>
+      <c r="P37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>69</v>
+      </c>
+      <c r="R37" t="s">
+        <v>69</v>
+      </c>
+      <c r="S37" t="s">
+        <v>69</v>
+      </c>
+      <c r="T37" t="s">
+        <v>69</v>
+      </c>
+      <c r="U37" t="s">
+        <v>69</v>
+      </c>
+      <c r="V37" t="s">
+        <v>69</v>
+      </c>
+      <c r="W37" t="s">
+        <v>69</v>
+      </c>
+      <c r="X37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC37" s="2">
+        <v>42235</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>43739</v>
+      </c>
+      <c r="AF37" s="3">
+        <v>43728</v>
+      </c>
+      <c r="AG37" s="2">
+        <v>43929</v>
+      </c>
+      <c r="AH37" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN37" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <v>47</v>
+      </c>
+      <c r="AR37">
+        <v>10</v>
+      </c>
+      <c r="AS37">
+        <v>6</v>
+      </c>
+      <c r="AT37">
+        <v>16</v>
+      </c>
+      <c r="AU37">
+        <v>31</v>
+      </c>
+      <c r="AV37" s="1">
+        <v>10</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>172</v>
+      </c>
+      <c r="AY37" t="s">
+        <v>124</v>
+      </c>
+      <c r="AZ37" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA37" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>88</v>
+      </c>
+      <c r="BC37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD37" t="s">
+        <v>147</v>
+      </c>
+      <c r="BE37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF37" t="s">
+        <v>90</v>
+      </c>
+      <c r="BG37" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH37" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="BJ37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK37" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL37" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN37" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO37" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP37" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ37" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>215</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>2030</v>
+      </c>
+      <c r="F38" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" t="s">
+        <v>70</v>
+      </c>
+      <c r="J38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" t="s">
+        <v>69</v>
+      </c>
+      <c r="N38" t="s">
+        <v>69</v>
+      </c>
+      <c r="O38" t="s">
+        <v>70</v>
+      </c>
+      <c r="P38" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>69</v>
+      </c>
+      <c r="R38" t="s">
+        <v>69</v>
+      </c>
+      <c r="S38" t="s">
+        <v>69</v>
+      </c>
+      <c r="T38" t="s">
+        <v>69</v>
+      </c>
+      <c r="U38" t="s">
+        <v>69</v>
+      </c>
+      <c r="V38" t="s">
+        <v>69</v>
+      </c>
+      <c r="W38" t="s">
+        <v>69</v>
+      </c>
+      <c r="X38" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC38" s="2">
+        <v>42310</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE38" s="2">
+        <v>43739</v>
+      </c>
+      <c r="AF38" s="3">
+        <v>43729</v>
+      </c>
+      <c r="AG38" s="2">
+        <v>43963</v>
+      </c>
+      <c r="AH38" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK38" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM38" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN38" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP38">
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <v>47</v>
+      </c>
+      <c r="AR38">
+        <v>16</v>
+      </c>
+      <c r="AS38">
+        <v>5</v>
+      </c>
+      <c r="AT38">
+        <v>29</v>
+      </c>
+      <c r="AU38">
+        <v>35</v>
+      </c>
+      <c r="AV38" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY38" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ38" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA38" t="s">
+        <v>146</v>
+      </c>
+      <c r="BB38" t="s">
+        <v>130</v>
+      </c>
+      <c r="BC38" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD38" t="s">
+        <v>92</v>
+      </c>
+      <c r="BE38" t="s">
+        <v>121</v>
+      </c>
+      <c r="BF38" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG38" t="s">
+        <v>147</v>
+      </c>
+      <c r="BH38" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BJ38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP38" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>2030</v>
+      </c>
+      <c r="F39" t="s">
+        <v>207</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39" t="s">
+        <v>70</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" t="s">
+        <v>69</v>
+      </c>
+      <c r="N39" t="s">
+        <v>69</v>
+      </c>
+      <c r="O39" t="s">
+        <v>70</v>
+      </c>
+      <c r="P39" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" t="s">
+        <v>69</v>
+      </c>
+      <c r="S39" t="s">
+        <v>69</v>
+      </c>
+      <c r="T39" t="s">
+        <v>69</v>
+      </c>
+      <c r="U39" t="s">
+        <v>69</v>
+      </c>
+      <c r="V39" t="s">
+        <v>69</v>
+      </c>
+      <c r="W39" t="s">
+        <v>69</v>
+      </c>
+      <c r="X39" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC39" s="2">
+        <v>42058</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE39" s="2">
+        <v>43739</v>
+      </c>
+      <c r="AF39" s="3">
+        <v>43729</v>
+      </c>
+      <c r="AG39" s="2">
+        <v>43963</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN39" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP39">
+        <v>5</v>
+      </c>
+      <c r="AQ39">
+        <v>52</v>
+      </c>
+      <c r="AR39">
+        <v>16</v>
+      </c>
+      <c r="AS39">
+        <v>16</v>
+      </c>
+      <c r="AT39">
+        <v>20</v>
+      </c>
+      <c r="AU39">
+        <v>33</v>
+      </c>
+      <c r="AV39" s="1">
+        <v>28</v>
+      </c>
+      <c r="AW39" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX39" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY39" t="s">
+        <v>88</v>
+      </c>
+      <c r="AZ39" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA39" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB39" t="s">
+        <v>89</v>
+      </c>
+      <c r="BC39" t="s">
+        <v>90</v>
+      </c>
+      <c r="BD39" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE39" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF39" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG39" t="s">
+        <v>138</v>
+      </c>
+      <c r="BH39" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI39" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BJ39" s="2">
+        <v>44741</v>
+      </c>
+      <c r="BK39" t="s">
+        <v>161</v>
+      </c>
+      <c r="BL39" t="s">
+        <v>95</v>
+      </c>
+      <c r="BM39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BN39" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO39" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP39" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>2030</v>
+      </c>
+      <c r="F40" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H40" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" t="s">
+        <v>70</v>
+      </c>
+      <c r="P40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" t="s">
+        <v>69</v>
+      </c>
+      <c r="S40" t="s">
+        <v>69</v>
+      </c>
+      <c r="T40" t="s">
+        <v>69</v>
+      </c>
+      <c r="U40" t="s">
+        <v>69</v>
+      </c>
+      <c r="V40" t="s">
+        <v>69</v>
+      </c>
+      <c r="W40" t="s">
+        <v>69</v>
+      </c>
+      <c r="X40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>42278</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>43739</v>
+      </c>
+      <c r="AF40" s="3">
+        <v>43729</v>
+      </c>
+      <c r="AG40" s="2">
+        <v>43999</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN40" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP40">
+        <v>0</v>
+      </c>
+      <c r="AQ40">
+        <v>44</v>
+      </c>
+      <c r="AR40">
+        <v>9</v>
+      </c>
+      <c r="AS40">
+        <v>3</v>
+      </c>
+      <c r="AT40">
+        <v>6</v>
+      </c>
+      <c r="AU40">
+        <v>19</v>
+      </c>
+      <c r="AV40" s="1">
+        <v>24</v>
+      </c>
+      <c r="AW40" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX40" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY40" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ40" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA40" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB40" t="s">
+        <v>129</v>
+      </c>
+      <c r="BC40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BE40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BH40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BI40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP40" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" t="s">
+        <v>215</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2030</v>
+      </c>
+      <c r="F41" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H41" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" t="s">
+        <v>69</v>
+      </c>
+      <c r="M41" t="s">
+        <v>69</v>
+      </c>
+      <c r="N41" t="s">
+        <v>69</v>
+      </c>
+      <c r="O41" t="s">
+        <v>70</v>
+      </c>
+      <c r="P41" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>69</v>
+      </c>
+      <c r="R41" t="s">
+        <v>69</v>
+      </c>
+      <c r="S41" t="s">
+        <v>69</v>
+      </c>
+      <c r="T41" t="s">
+        <v>69</v>
+      </c>
+      <c r="U41" t="s">
+        <v>69</v>
+      </c>
+      <c r="V41" t="s">
+        <v>69</v>
+      </c>
+      <c r="W41" t="s">
+        <v>69</v>
+      </c>
+      <c r="X41" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC41" s="2">
+        <v>42450</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE41" s="2">
+        <v>44972</v>
+      </c>
+      <c r="AF41" s="3">
+        <v>44967</v>
+      </c>
+      <c r="AG41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN41" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP41">
+        <v>0</v>
+      </c>
+      <c r="AQ41">
+        <v>29</v>
+      </c>
+      <c r="AR41">
+        <v>6</v>
+      </c>
+      <c r="AS41">
+        <v>0</v>
+      </c>
+      <c r="AT41">
+        <v>4</v>
+      </c>
+      <c r="AU41">
+        <v>8</v>
+      </c>
+      <c r="AV41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY41" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BB41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BE41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BH41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BI41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP41" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR41" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="F1:F36" xr:uid="{01BC0FAF-0515-DD4A-8720-9B9E6959245E}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Sort masterfile for reporting
</commit_message>
<xml_diff>
--- a/tests/data/example_masterfile.xlsx
+++ b/tests/data/example_masterfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiebuntic/projects/RRED/rred-reports/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/rred-reports/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17ED436-6FD4-D343-A477-2DC23E409698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB2BC22-D4D4-A94F-B74F-47D8BFF99187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,28 +665,28 @@
     <t>J School</t>
   </si>
   <si>
-    <t>test-1_2021-22</t>
-  </si>
-  <si>
-    <t>test-2_2021-22</t>
-  </si>
-  <si>
-    <t>test-3_2021-22</t>
-  </si>
-  <si>
-    <t>test-4_2021-22</t>
-  </si>
-  <si>
-    <t>test-5_2021-22</t>
-  </si>
-  <si>
-    <t>test-6_2021-22</t>
-  </si>
-  <si>
     <t>Left School</t>
   </si>
   <si>
     <t>AF066XX</t>
+  </si>
+  <si>
+    <t>1_2021-22-test</t>
+  </si>
+  <si>
+    <t>2_2021-22-test</t>
+  </si>
+  <si>
+    <t>3_2021-22-test</t>
+  </si>
+  <si>
+    <t>4_2021-22-test</t>
+  </si>
+  <si>
+    <t>5_2021-22-test</t>
+  </si>
+  <si>
+    <t>11_2021-22-test</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:BR41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
         <v>187</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
         <v>187</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
         <v>187</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
         <v>187</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
         <v>187</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
         <v>187</v>
@@ -2855,7 +2855,7 @@
         <v>69</v>
       </c>
       <c r="AH9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="AI9" t="s">
         <v>112</v>
@@ -8620,7 +8620,7 @@
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
         <v>81</v>
@@ -8829,7 +8829,7 @@
         <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
         <v>81</v>
@@ -9038,7 +9038,7 @@
         <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C39" t="s">
         <v>81</v>
@@ -9247,7 +9247,7 @@
         <v>111</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
         <v>81</v>
@@ -9459,7 +9459,7 @@
         <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s">
         <v>81</v>

</xml_diff>